<commit_message>
Add parallel implementation using MPI
</commit_message>
<xml_diff>
--- a/Documentation/Execution timings.xlsx
+++ b/Documentation/Execution timings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultate\Anul III\Algoritmi Paraleli si Distribuiti\Parallel and Distributed Algorithms Project\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultate\Anul III\Algoritmi Paraleli si Distribuiti\PDA Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8925D2F-32B5-450E-9324-7487434EAC73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60244772-781B-411A-8FB7-61D0DC04AF0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Sequential</t>
   </si>
@@ -33,13 +33,34 @@
     <t>Test Size</t>
   </si>
   <si>
-    <t>Parallel 1</t>
-  </si>
-  <si>
     <t>Parallel 2</t>
   </si>
   <si>
     <t>Application Runtime (seconds)</t>
+  </si>
+  <si>
+    <t>Parallel MPI</t>
+  </si>
+  <si>
+    <t>2 processes</t>
+  </si>
+  <si>
+    <t>5 processes</t>
+  </si>
+  <si>
+    <t>8 processes</t>
+  </si>
+  <si>
+    <t>10 processes</t>
+  </si>
+  <si>
+    <t>16 processes</t>
+  </si>
+  <si>
+    <t>20 processes</t>
+  </si>
+  <si>
+    <t>50 processes</t>
   </si>
 </sst>
 </file>
@@ -138,8 +159,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sequential Implementation</a:t>
+              <a:t>Sequantial</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> VS MPI</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -331,6 +357,153 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Parallel MPI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0519999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.186999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.889000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76.593999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7874-4F2A-812A-DC549B2178FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -344,6 +517,1349 @@
       </c:scatterChart>
       <c:valAx>
         <c:axId val="740440224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740437312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="740437312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740440224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Parallel</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Implementation using MPI</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5009999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2480000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.067</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B7B-4A26-B3F8-B6A49214F6C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5 processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1289999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.166</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.409999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79.257999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0B7B-4A26-B3F8-B6A49214F6C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$3:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9770000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0780000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.364000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.761000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.492000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0B7B-4A26-B3F8-B6A49214F6C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10 processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9330000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0519999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.186999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.889000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76.593999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0B7B-4A26-B3F8-B6A49214F6C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8979999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.332000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.249000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.730999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0B7B-4A26-B3F8-B6A49214F6C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20 processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.132</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.048999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79.402000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0B7B-4A26-B3F8-B6A49214F6C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50 processes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$3:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$3:$N$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.624000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.386000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81.058000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-0B7B-4A26-B3F8-B6A49214F6C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1427789984"/>
+        <c:axId val="1427784576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1427789984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -383,7 +1899,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Test size</a:t>
+                  <a:t>tEST SIZE</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -450,12 +1966,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="740437312"/>
+        <c:crossAx val="1427784576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="740437312"/>
+        <c:axId val="1427784576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +2011,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time in seconds</a:t>
+                  <a:t>TIME IN SECONDS</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -562,7 +2078,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="740440224"/>
+        <c:crossAx val="1427789984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -574,6 +2090,36 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -659,6 +2205,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
@@ -1161,20 +2747,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1194,6 +3282,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE443D1A-D431-4530-89F3-BCF1DEFA606A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1465,26 +3589,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1492,79 +3628,320 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100</v>
       </c>
       <c r="B3">
         <v>2E-3</v>
       </c>
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N3">
+        <v>8.9999999999999993E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000</v>
       </c>
       <c r="B4">
         <v>2.9000000000000001E-2</v>
       </c>
+      <c r="C4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="G4">
+        <v>1000</v>
+      </c>
+      <c r="H4">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="I4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J4">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="L4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="M4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="N4">
+        <v>3.2000000000000001E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10000</v>
       </c>
       <c r="B5">
         <v>0.33700000000000002</v>
       </c>
+      <c r="C5">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="G5">
+        <v>10000</v>
+      </c>
+      <c r="H5">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="I5">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="J5">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="K5">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="L5">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="M5">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="N5">
+        <v>0.35099999999999998</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50000</v>
       </c>
       <c r="B6">
         <v>1.847</v>
       </c>
+      <c r="C6">
+        <v>1.9330000000000001</v>
+      </c>
+      <c r="G6">
+        <v>50000</v>
+      </c>
+      <c r="H6">
+        <v>2.5009999999999999</v>
+      </c>
+      <c r="I6">
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="J6">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="K6">
+        <v>1.9330000000000001</v>
+      </c>
+      <c r="L6">
+        <v>1.8979999999999999</v>
+      </c>
+      <c r="M6">
+        <v>1.8959999999999999</v>
+      </c>
+      <c r="N6">
+        <v>1.998</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>100000</v>
       </c>
       <c r="B7">
         <v>3.85</v>
       </c>
+      <c r="C7">
+        <v>4.0519999999999996</v>
+      </c>
+      <c r="G7">
+        <v>100000</v>
+      </c>
+      <c r="H7">
+        <v>5.2480000000000002</v>
+      </c>
+      <c r="I7">
+        <v>4.1289999999999996</v>
+      </c>
+      <c r="J7">
+        <v>4.0780000000000003</v>
+      </c>
+      <c r="K7">
+        <v>4.0519999999999996</v>
+      </c>
+      <c r="L7">
+        <v>3.94</v>
+      </c>
+      <c r="M7">
+        <v>3.9180000000000001</v>
+      </c>
+      <c r="N7">
+        <v>4.1159999999999997</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>300000</v>
       </c>
       <c r="B8">
         <v>14.316000000000001</v>
       </c>
+      <c r="C8">
+        <v>14.186999999999999</v>
+      </c>
+      <c r="G8">
+        <v>300000</v>
+      </c>
+      <c r="H8">
+        <v>18.375</v>
+      </c>
+      <c r="I8">
+        <v>15.166</v>
+      </c>
+      <c r="J8">
+        <v>14.364000000000001</v>
+      </c>
+      <c r="K8">
+        <v>14.186999999999999</v>
+      </c>
+      <c r="L8">
+        <v>14.332000000000001</v>
+      </c>
+      <c r="M8">
+        <v>14.132</v>
+      </c>
+      <c r="N8">
+        <v>14.624000000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>600000</v>
       </c>
       <c r="B9">
         <v>36.862000000000002</v>
       </c>
+      <c r="C9">
+        <v>35.889000000000003</v>
+      </c>
+      <c r="G9">
+        <v>600000</v>
+      </c>
+      <c r="H9">
+        <v>45.067</v>
+      </c>
+      <c r="I9">
+        <v>38.409999999999997</v>
+      </c>
+      <c r="J9">
+        <v>36.761000000000003</v>
+      </c>
+      <c r="K9">
+        <v>35.889000000000003</v>
+      </c>
+      <c r="L9">
+        <v>36.249000000000002</v>
+      </c>
+      <c r="M9">
+        <v>35.048999999999999</v>
+      </c>
+      <c r="N9">
+        <v>36.386000000000003</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1000000</v>
       </c>
       <c r="B10">
         <v>78.524000000000001</v>
       </c>
+      <c r="C10">
+        <v>76.593999999999994</v>
+      </c>
+      <c r="G10">
+        <v>1000000</v>
+      </c>
+      <c r="H10">
+        <v>91.12</v>
+      </c>
+      <c r="I10">
+        <v>79.257999999999996</v>
+      </c>
+      <c r="J10">
+        <v>78.492000000000004</v>
+      </c>
+      <c r="K10">
+        <v>76.593999999999994</v>
+      </c>
+      <c r="L10">
+        <v>78.730999999999995</v>
+      </c>
+      <c r="M10">
+        <v>79.402000000000001</v>
+      </c>
+      <c r="N10">
+        <v>81.058000000000007</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update parallel MPI implementation
</commit_message>
<xml_diff>
--- a/Documentation/Execution timings.xlsx
+++ b/Documentation/Execution timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultate\Anul III\Algoritmi Paraleli si Distribuiti\PDA Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60244772-781B-411A-8FB7-61D0DC04AF0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9CDDA2-2546-4549-9BDA-B0E45465664C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>16 processes</t>
   </si>
   <si>
-    <t>20 processes</t>
+    <t>32 processes</t>
   </si>
   <si>
-    <t>50 processes</t>
+    <t>64 processes</t>
   </si>
 </sst>
 </file>
@@ -471,28 +471,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35399999999999998</c:v>
+                  <c:v>6.6000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9330000000000001</c:v>
+                  <c:v>0.29499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0519999999999996</c:v>
+                  <c:v>0.68899999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.186999999999999</c:v>
+                  <c:v>3.7029999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.889000000000003</c:v>
+                  <c:v>12.714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>76.593999999999994</c:v>
+                  <c:v>32.533999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -925,28 +925,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0999999999999997E-2</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45300000000000001</c:v>
+                  <c:v>0.16700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5009999999999999</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2480000000000002</c:v>
+                  <c:v>1.7629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.375</c:v>
+                  <c:v>7.5830000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.067</c:v>
+                  <c:v>20.824000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>91.12</c:v>
+                  <c:v>47.517000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1075,25 +1075,25 @@
                   <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7999999999999999E-2</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36399999999999999</c:v>
+                  <c:v>9.6000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9950000000000001</c:v>
+                  <c:v>0.51800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1289999999999996</c:v>
+                  <c:v>1.1040000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.166</c:v>
+                  <c:v>4.9790000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.409999999999997</c:v>
+                  <c:v>15.752000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79.257999999999996</c:v>
+                  <c:v>37.817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1219,28 +1219,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36599999999999999</c:v>
+                  <c:v>6.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9770000000000001</c:v>
+                  <c:v>0.32200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0780000000000003</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.364000000000001</c:v>
+                  <c:v>4.024</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.761000000000003</c:v>
+                  <c:v>13.387</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>78.492000000000004</c:v>
+                  <c:v>33.959000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1366,28 +1366,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35399999999999998</c:v>
+                  <c:v>6.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9330000000000001</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0519999999999996</c:v>
+                  <c:v>0.84699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.186999999999999</c:v>
+                  <c:v>4.0629999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.889000000000003</c:v>
+                  <c:v>13.49</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>76.593999999999994</c:v>
+                  <c:v>34.146000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,28 +1513,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4000000000000002E-2</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35299999999999998</c:v>
+                  <c:v>6.6000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8979999999999999</c:v>
+                  <c:v>0.29499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.94</c:v>
+                  <c:v>0.68899999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.332000000000001</c:v>
+                  <c:v>3.7029999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.249000000000002</c:v>
+                  <c:v>12.714</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>78.730999999999995</c:v>
+                  <c:v>32.533999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1555,7 +1555,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20 processes</c:v>
+                  <c:v>32 processes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1660,28 +1660,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5000000000000003E-2</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34699999999999998</c:v>
+                  <c:v>5.8000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8959999999999999</c:v>
+                  <c:v>0.30099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9180000000000001</c:v>
+                  <c:v>0.69799999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.132</c:v>
+                  <c:v>3.6850000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.048999999999999</c:v>
+                  <c:v>12.795</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79.402000000000001</c:v>
+                  <c:v>33.406999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1702,7 +1702,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50 processes</c:v>
+                  <c:v>64 processes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1814,28 +1814,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8.9999999999999993E-3</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35099999999999998</c:v>
+                  <c:v>6.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.998</c:v>
+                  <c:v>0.32300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1159999999999997</c:v>
+                  <c:v>0.69299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.624000000000001</c:v>
+                  <c:v>3.718</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.386000000000003</c:v>
+                  <c:v>13.005000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81.058000000000007</c:v>
+                  <c:v>32.86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3592,7 +3592,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3603,6 +3603,7 @@
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -3666,31 +3667,31 @@
         <v>2E-3</v>
       </c>
       <c r="C3">
-        <v>0.05</v>
+        <v>2E-3</v>
       </c>
       <c r="G3">
         <v>100</v>
       </c>
       <c r="H3">
-        <v>4.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="I3">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="J3">
+        <v>2E-3</v>
+      </c>
+      <c r="K3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L3">
+        <v>2E-3</v>
+      </c>
+      <c r="M3">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K3">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="L3">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="M3">
-        <v>8.0000000000000002E-3</v>
-      </c>
       <c r="N3">
-        <v>8.9999999999999993E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3701,31 +3702,31 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="C4">
-        <v>3.1E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="G4">
         <v>1000</v>
       </c>
       <c r="H4">
-        <v>5.0999999999999997E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I4">
-        <v>3.7999999999999999E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="J4">
-        <v>3.2000000000000001E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="K4">
-        <v>3.1E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="L4">
-        <v>3.4000000000000002E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="M4">
-        <v>3.5000000000000003E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N4">
-        <v>3.2000000000000001E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -3736,31 +3737,31 @@
         <v>0.33700000000000002</v>
       </c>
       <c r="C5">
-        <v>0.35399999999999998</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="G5">
         <v>10000</v>
       </c>
       <c r="H5">
-        <v>0.45300000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="I5">
-        <v>0.36399999999999999</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="J5">
-        <v>0.36599999999999999</v>
+        <v>6.3E-2</v>
       </c>
       <c r="K5">
-        <v>0.35399999999999998</v>
+        <v>6.3E-2</v>
       </c>
       <c r="L5">
-        <v>0.35299999999999998</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="M5">
-        <v>0.34699999999999998</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="N5">
-        <v>0.35099999999999998</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -3771,31 +3772,31 @@
         <v>1.847</v>
       </c>
       <c r="C6">
-        <v>1.9330000000000001</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="G6">
         <v>50000</v>
       </c>
       <c r="H6">
-        <v>2.5009999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="I6">
-        <v>1.9950000000000001</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="J6">
-        <v>1.9770000000000001</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="K6">
-        <v>1.9330000000000001</v>
+        <v>0.34</v>
       </c>
       <c r="L6">
-        <v>1.8979999999999999</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="M6">
-        <v>1.8959999999999999</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="N6">
-        <v>1.998</v>
+        <v>0.32300000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -3806,31 +3807,31 @@
         <v>3.85</v>
       </c>
       <c r="C7">
-        <v>4.0519999999999996</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="G7">
         <v>100000</v>
       </c>
       <c r="H7">
-        <v>5.2480000000000002</v>
+        <v>1.7629999999999999</v>
       </c>
       <c r="I7">
-        <v>4.1289999999999996</v>
+        <v>1.1040000000000001</v>
       </c>
       <c r="J7">
-        <v>4.0780000000000003</v>
+        <v>0.88</v>
       </c>
       <c r="K7">
-        <v>4.0519999999999996</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="L7">
-        <v>3.94</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="M7">
-        <v>3.9180000000000001</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="N7">
-        <v>4.1159999999999997</v>
+        <v>0.69299999999999995</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3841,31 +3842,31 @@
         <v>14.316000000000001</v>
       </c>
       <c r="C8">
-        <v>14.186999999999999</v>
+        <v>3.7029999999999998</v>
       </c>
       <c r="G8">
         <v>300000</v>
       </c>
       <c r="H8">
-        <v>18.375</v>
+        <v>7.5830000000000002</v>
       </c>
       <c r="I8">
-        <v>15.166</v>
+        <v>4.9790000000000001</v>
       </c>
       <c r="J8">
-        <v>14.364000000000001</v>
+        <v>4.024</v>
       </c>
       <c r="K8">
-        <v>14.186999999999999</v>
+        <v>4.0629999999999997</v>
       </c>
       <c r="L8">
-        <v>14.332000000000001</v>
+        <v>3.7029999999999998</v>
       </c>
       <c r="M8">
-        <v>14.132</v>
+        <v>3.6850000000000001</v>
       </c>
       <c r="N8">
-        <v>14.624000000000001</v>
+        <v>3.718</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -3876,31 +3877,31 @@
         <v>36.862000000000002</v>
       </c>
       <c r="C9">
-        <v>35.889000000000003</v>
+        <v>12.714</v>
       </c>
       <c r="G9">
         <v>600000</v>
       </c>
       <c r="H9">
-        <v>45.067</v>
+        <v>20.824000000000002</v>
       </c>
       <c r="I9">
-        <v>38.409999999999997</v>
+        <v>15.752000000000001</v>
       </c>
       <c r="J9">
-        <v>36.761000000000003</v>
+        <v>13.387</v>
       </c>
       <c r="K9">
-        <v>35.889000000000003</v>
+        <v>13.49</v>
       </c>
       <c r="L9">
-        <v>36.249000000000002</v>
+        <v>12.714</v>
       </c>
       <c r="M9">
-        <v>35.048999999999999</v>
+        <v>12.795</v>
       </c>
       <c r="N9">
-        <v>36.386000000000003</v>
+        <v>13.005000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -3911,31 +3912,31 @@
         <v>78.524000000000001</v>
       </c>
       <c r="C10">
-        <v>76.593999999999994</v>
+        <v>32.533999999999999</v>
       </c>
       <c r="G10">
         <v>1000000</v>
       </c>
       <c r="H10">
-        <v>91.12</v>
+        <v>47.517000000000003</v>
       </c>
       <c r="I10">
-        <v>79.257999999999996</v>
+        <v>37.817</v>
       </c>
       <c r="J10">
-        <v>78.492000000000004</v>
+        <v>33.959000000000003</v>
       </c>
       <c r="K10">
-        <v>76.593999999999994</v>
+        <v>34.146000000000001</v>
       </c>
       <c r="L10">
-        <v>78.730999999999995</v>
+        <v>32.533999999999999</v>
       </c>
       <c r="M10">
-        <v>79.402000000000001</v>
+        <v>33.406999999999996</v>
       </c>
       <c r="N10">
-        <v>81.058000000000007</v>
+        <v>32.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add parallel implementation using C++ Threads
</commit_message>
<xml_diff>
--- a/Documentation/Execution timings.xlsx
+++ b/Documentation/Execution timings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultate\Anul III\Algoritmi Paraleli si Distribuiti\PDA Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9CDDA2-2546-4549-9BDA-B0E45465664C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF26E9A2-6FA8-4C6D-879C-DCD5E80CE21F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Sequential</t>
   </si>
   <si>
     <t>Test Size</t>
-  </si>
-  <si>
-    <t>Parallel 2</t>
   </si>
   <si>
     <t>Application Runtime (seconds)</t>
@@ -61,6 +58,36 @@
   </si>
   <si>
     <t>64 processes</t>
+  </si>
+  <si>
+    <t>Application Runtime (seconds) - MPI</t>
+  </si>
+  <si>
+    <t>Application Runtime (seconds) - C++ Threads</t>
+  </si>
+  <si>
+    <t>2 threads</t>
+  </si>
+  <si>
+    <t>5 threads</t>
+  </si>
+  <si>
+    <t>8 threads</t>
+  </si>
+  <si>
+    <t>10 threads</t>
+  </si>
+  <si>
+    <t>16 threads</t>
+  </si>
+  <si>
+    <t>32 threads</t>
+  </si>
+  <si>
+    <t>64 threads</t>
+  </si>
+  <si>
+    <t>Parallel C++ Threads</t>
   </si>
 </sst>
 </file>
@@ -159,11 +186,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sequantial</a:t>
+              <a:t>Sequential vs </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> VS MPI</a:t>
+              <a:t>MPI vs C++ Threads</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -501,6 +528,153 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7874-4F2A-812A-DC549B2178FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Parallel C++ Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80300000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0760000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0791-4104-8782-1A1DB5626769}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1844,6 +2018,1437 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-0B7B-4A26-B3F8-B6A49214F6C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1427789984"/>
+        <c:axId val="1427784576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1427789984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>tEST SIZE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1427784576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1427784576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>TIME IN SECONDS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1427789984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Parallel</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Implementation using C++ Threads</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$15:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.41899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80300000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0760000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-623D-4907-B33F-B28A1F1F9B38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5 threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$15:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.435</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4209999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7869999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-623D-4907-B33F-B28A1F1F9B38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8 threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$15:$J$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.593</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9820000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.2170000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-623D-4907-B33F-B28A1F1F9B38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10 threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$15:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.9000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.44800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.80300000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.393</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5309999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.734</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-623D-4907-B33F-B28A1F1F9B38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16 threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$15:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5519999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.946000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.190999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.827000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-623D-4907-B33F-B28A1F1F9B38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>32 threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$15:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.121</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8289999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.798000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.974000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-623D-4907-B33F-B28A1F1F9B38}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64 threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$15:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$15:$N$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9.9000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.497999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.141000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-623D-4907-B33F-B28A1F1F9B38}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2245,6 +3850,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
@@ -2748,6 +4393,508 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3318,6 +5465,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>33339</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AA25A4D-C562-410A-8710-90D7C15E4145}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3589,10 +5774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3600,6 +5785,7 @@
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="12.140625" bestFit="1" customWidth="1"/>
@@ -3608,12 +5794,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -3629,34 +5815,34 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>10</v>
-      </c>
-      <c r="N2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -3669,6 +5855,9 @@
       <c r="C3">
         <v>2E-3</v>
       </c>
+      <c r="D3">
+        <v>5.0000000000000001E-3</v>
+      </c>
       <c r="G3">
         <v>100</v>
       </c>
@@ -3704,6 +5893,9 @@
       <c r="C4">
         <v>6.0000000000000001E-3</v>
       </c>
+      <c r="D4">
+        <v>1.0999999999999999E-2</v>
+      </c>
       <c r="G4">
         <v>1000</v>
       </c>
@@ -3739,6 +5931,9 @@
       <c r="C5">
         <v>6.6000000000000003E-2</v>
       </c>
+      <c r="D5">
+        <v>8.1000000000000003E-2</v>
+      </c>
       <c r="G5">
         <v>10000</v>
       </c>
@@ -3774,6 +5969,9 @@
       <c r="C6">
         <v>0.29499999999999998</v>
       </c>
+      <c r="D6">
+        <v>0.41899999999999998</v>
+      </c>
       <c r="G6">
         <v>50000</v>
       </c>
@@ -3809,6 +6007,9 @@
       <c r="C7">
         <v>0.68899999999999995</v>
       </c>
+      <c r="D7">
+        <v>0.80300000000000005</v>
+      </c>
       <c r="G7">
         <v>100000</v>
       </c>
@@ -3844,6 +6045,9 @@
       <c r="C8">
         <v>3.7029999999999998</v>
       </c>
+      <c r="D8">
+        <v>2.4</v>
+      </c>
       <c r="G8">
         <v>300000</v>
       </c>
@@ -3879,6 +6083,9 @@
       <c r="C9">
         <v>12.714</v>
       </c>
+      <c r="D9">
+        <v>4.78</v>
+      </c>
       <c r="G9">
         <v>600000</v>
       </c>
@@ -3914,6 +6121,9 @@
       <c r="C10">
         <v>32.533999999999999</v>
       </c>
+      <c r="D10">
+        <v>8.0760000000000005</v>
+      </c>
       <c r="G10">
         <v>1000000</v>
       </c>
@@ -3939,10 +6149,237 @@
         <v>32.86</v>
       </c>
     </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I15">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J15">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="K15">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="L15">
+        <v>0.13</v>
+      </c>
+      <c r="M15">
+        <v>0.121</v>
+      </c>
+      <c r="N15">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>1000</v>
+      </c>
+      <c r="H16">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J16">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="K16">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="L16">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="M16">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="N16">
+        <v>0.66200000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>10000</v>
+      </c>
+      <c r="H17">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="I17">
+        <v>0.1</v>
+      </c>
+      <c r="J17">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="K17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L17">
+        <v>6.5519999999999996</v>
+      </c>
+      <c r="M17">
+        <v>6.8289999999999997</v>
+      </c>
+      <c r="N17">
+        <v>6.4630000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>50000</v>
+      </c>
+      <c r="H18">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="I18">
+        <v>0.435</v>
+      </c>
+      <c r="J18">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="K18">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="L18">
+        <v>23.122</v>
+      </c>
+      <c r="M18">
+        <v>34.798000000000002</v>
+      </c>
+      <c r="N18">
+        <v>34.497999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>100000</v>
+      </c>
+      <c r="H19">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="I19">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="J19">
+        <v>1.02</v>
+      </c>
+      <c r="K19">
+        <v>1.393</v>
+      </c>
+      <c r="L19">
+        <v>22.85</v>
+      </c>
+      <c r="M19">
+        <v>67.974000000000004</v>
+      </c>
+      <c r="N19">
+        <v>70.141000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>300000</v>
+      </c>
+      <c r="H20">
+        <v>2.4</v>
+      </c>
+      <c r="I20">
+        <v>2.4209999999999998</v>
+      </c>
+      <c r="J20">
+        <v>2.593</v>
+      </c>
+      <c r="K20">
+        <v>3.0369999999999999</v>
+      </c>
+      <c r="L20">
+        <v>25.946000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>600000</v>
+      </c>
+      <c r="H21">
+        <v>4.78</v>
+      </c>
+      <c r="I21">
+        <v>4.7869999999999999</v>
+      </c>
+      <c r="J21">
+        <v>4.9820000000000002</v>
+      </c>
+      <c r="K21">
+        <v>5.5309999999999997</v>
+      </c>
+      <c r="L21">
+        <v>27.190999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>1000000</v>
+      </c>
+      <c r="H22">
+        <v>8.0760000000000005</v>
+      </c>
+      <c r="I22">
+        <v>8.11</v>
+      </c>
+      <c r="J22">
+        <v>8.2170000000000005</v>
+      </c>
+      <c r="K22">
+        <v>8.734</v>
+      </c>
+      <c r="L22">
+        <v>30.827000000000002</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="H1:M1"/>
+    <mergeCell ref="H13:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>